<commit_message>
Latest changes - Pages, Testcases, Test Data, packaes - 15th Mar 2023
</commit_message>
<xml_diff>
--- a/TestData/TMTC0019612_VerifyExternalContactFeaturesOnSFLightning.xlsx
+++ b/TestData/TMTC0019612_VerifyExternalContactFeaturesOnSFLightning.xlsx
@@ -8,16 +8,18 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\HL\SF_Automation\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D6EAD585-E3D6-4538-A5D3-21A798FED03C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FFE387A3-7EF4-4B77-ABD0-F8D7904F9651}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Users" sheetId="2" r:id="rId1"/>
-    <sheet name="RecentlyViewedListView" sheetId="5" r:id="rId2"/>
-    <sheet name="Activity" sheetId="4" r:id="rId3"/>
-    <sheet name="Contact" sheetId="6" r:id="rId4"/>
-    <sheet name="ContactTypes" sheetId="7" r:id="rId5"/>
+    <sheet name="QuickLinks" sheetId="8" r:id="rId2"/>
+    <sheet name="AddRelationship" sheetId="9" r:id="rId3"/>
+    <sheet name="RecentlyViewedListView" sheetId="5" r:id="rId4"/>
+    <sheet name="Activity" sheetId="4" r:id="rId5"/>
+    <sheet name="Contact" sheetId="6" r:id="rId6"/>
+    <sheet name="ContactTypes" sheetId="7" r:id="rId7"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -29,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="53">
   <si>
     <t>Users</t>
   </si>
@@ -122,6 +124,72 @@
   </si>
   <si>
     <t>External Contact</t>
+  </si>
+  <si>
+    <t>QuickLinkNames</t>
+  </si>
+  <si>
+    <t>HL Relationships</t>
+  </si>
+  <si>
+    <t>Industry Focus</t>
+  </si>
+  <si>
+    <t>Opportunity Contacts</t>
+  </si>
+  <si>
+    <t>Engagements Shown</t>
+  </si>
+  <si>
+    <t>Affiliated Companies</t>
+  </si>
+  <si>
+    <t>Memberships</t>
+  </si>
+  <si>
+    <t>Contact Sectors</t>
+  </si>
+  <si>
+    <t>Campaign History</t>
+  </si>
+  <si>
+    <t>Contact Email History</t>
+  </si>
+  <si>
+    <t>Contact Sources</t>
+  </si>
+  <si>
+    <t>Development Leads</t>
+  </si>
+  <si>
+    <t>Files</t>
+  </si>
+  <si>
+    <t>Contact History</t>
+  </si>
+  <si>
+    <t>Engagements Contacts</t>
+  </si>
+  <si>
+    <t>Strength Rating</t>
+  </si>
+  <si>
+    <t>Lookup Employee</t>
+  </si>
+  <si>
+    <t>Type</t>
+  </si>
+  <si>
+    <t>Personal Note</t>
+  </si>
+  <si>
+    <t>Outlook Categories</t>
+  </si>
+  <si>
+    <t>High</t>
+  </si>
+  <si>
+    <t>Business</t>
   </si>
 </sst>
 </file>
@@ -491,6 +559,156 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7972DAA3-2502-4122-BD46-655C1E9DC13D}">
+  <dimension ref="A1:A15"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F14" sqref="F14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="19.6640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="14" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="15" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>44</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2F3F8239-6B74-44DC-BFBB-805C79460C38}">
+  <dimension ref="A1:E2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E2" sqref="E2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="16.21875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.77734375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.21875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B2" t="s">
+        <v>51</v>
+      </c>
+      <c r="C2" t="s">
+        <v>52</v>
+      </c>
+      <c r="D2" t="s">
+        <v>25</v>
+      </c>
+      <c r="E2" t="s">
+        <v>25</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{238E81D2-2BA2-4C65-87A5-507061E9159C}">
   <dimension ref="A1:A8"/>
   <sheetViews>
@@ -549,7 +767,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:F2"/>
   <sheetViews>
@@ -599,7 +817,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{539639EE-7BFC-4886-96EB-3951B3718C01}">
   <dimension ref="A1:E2"/>
   <sheetViews>
@@ -658,11 +876,11 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B9C49F78-6D2A-46C0-BDF2-39A2D491D8C0}">
   <dimension ref="A1:A2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
LV Contacts - 11 July 2024
</commit_message>
<xml_diff>
--- a/TestData/TMTC0019612_VerifyExternalContactFeaturesOnSFLightning.xlsx
+++ b/TestData/TMTC0019612_VerifyExternalContactFeaturesOnSFLightning.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27726"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\HL\SF_Automation\TestData\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SMittal0207\source\repos\SF_Automation\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FFE387A3-7EF4-4B77-ABD0-F8D7904F9651}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{03D74864-E144-4AB2-BD32-79668912507C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Users" sheetId="2" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="55">
   <si>
     <t>Users</t>
   </si>
@@ -190,6 +190,12 @@
   </si>
   <si>
     <t>Business</t>
+  </si>
+  <si>
+    <t>ContactName</t>
+  </si>
+  <si>
+    <t>Test LVContact</t>
   </si>
 </sst>
 </file>
@@ -656,7 +662,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2F3F8239-6B74-44DC-BFBB-805C79460C38}">
   <dimension ref="A1:E2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
@@ -819,10 +825,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{539639EE-7BFC-4886-96EB-3951B3718C01}">
-  <dimension ref="A1:E2"/>
+  <dimension ref="A1:F2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E24" sqref="E24"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -832,9 +838,10 @@
     <col min="3" max="3" width="14.33203125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="13.33203125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="18.33203125" customWidth="1"/>
+    <col min="6" max="6" width="13.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>20</v>
       </c>
@@ -850,8 +857,11 @@
       <c r="E1" s="1" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F1" s="1" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -866,6 +876,9 @@
       </c>
       <c r="E2" s="4" t="s">
         <v>28</v>
+      </c>
+      <c r="F2" t="s">
+        <v>54</v>
       </c>
     </row>
   </sheetData>

</xml_diff>